<commit_message>
Header 변경 및 WBS 수정
</commit_message>
<xml_diff>
--- a/WBS_Pro01_작업자,일정 표시 필요.xlsx
+++ b/WBS_Pro01_작업자,일정 표시 필요.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\project\Chunjae_Team_Proj01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlsdp\Desktop\github\Chunjae_Team_Proj01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA26CF7-9957-46CF-8580-6A432B459D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFDBA7F-7C81-4E67-AE75-FE808212B220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="187">
   <si>
     <t>프로젝트 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -492,35 +492,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4. 소개 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. 게시판 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.3 FAQ 게시판 HTML5+CSS3 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.4 공지사항 게시판 HTML5+CSS3 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>백엔드 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1 학부모 커뮤니티 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1 회사 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2 서비스 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -569,10 +541,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.2 Q&amp;A 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.1 메인페이지 각 페이지 요소 별 JSP 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -724,6 +692,58 @@
   </si>
   <si>
     <t>신예은, 김보경, 김현경, 박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 관리자 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 소개 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 게시판 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1 회사 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2 서비스 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.1 학부모 커뮤니티 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2 Q&amp;A 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.3 FAQ 게시판 HTML5+CSS3 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.4 공지사항 게시판 HTML5+CSS3 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-1. 관리자 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2. 회원관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-3. 고객지원 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-4. 게시판 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -844,7 +864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1069,19 +1089,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1097,19 +1104,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1376,95 +1370,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border diagonalUp="1" diagonalDown="1">
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal style="medium">
         <color indexed="64"/>
       </diagonal>
     </border>
     <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal style="medium">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="medium">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal style="medium">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1473,7 +1507,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1519,88 +1553,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1609,40 +1631,73 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1654,166 +1709,208 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2130,319 +2227,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:BW72"/>
+  <dimension ref="B2:BW76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="57.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.83203125" style="4" customWidth="1"/>
     <col min="7" max="10" width="8.75" style="4"/>
-    <col min="11" max="11" width="18.125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="18.08203125" style="4" customWidth="1"/>
     <col min="12" max="12" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="71" width="4.75" style="4" customWidth="1"/>
     <col min="72" max="75" width="4.75" style="1" customWidth="1"/>
     <col min="76" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="64"/>
+      <c r="E2" s="80"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="64"/>
+      <c r="E3" s="80"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="80"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="64"/>
+      <c r="E5" s="80"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="64"/>
-    </row>
-    <row r="7" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="E6" s="80"/>
+    </row>
+    <row r="7" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="64" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="64"/>
-    </row>
-    <row r="9" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65"/>
-    <row r="10" spans="2:75" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="80" t="s">
+      <c r="D7" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="80"/>
+    </row>
+    <row r="9" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="2:75" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="69" t="s">
+      <c r="K10" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="78" t="s">
+      <c r="L10" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="72" t="s">
-        <v>179</v>
-      </c>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
-      <c r="U10" s="72"/>
-      <c r="V10" s="72"/>
-      <c r="W10" s="72"/>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="72"/>
-      <c r="Z10" s="72"/>
-      <c r="AA10" s="72"/>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="72"/>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="72"/>
-      <c r="AG10" s="72"/>
-      <c r="AH10" s="72"/>
-      <c r="AI10" s="72"/>
-      <c r="AJ10" s="72"/>
-      <c r="AK10" s="72"/>
-      <c r="AL10" s="72"/>
-      <c r="AM10" s="72"/>
-      <c r="AN10" s="72"/>
-      <c r="AO10" s="72"/>
-      <c r="AP10" s="72"/>
-      <c r="AQ10" s="72"/>
-      <c r="AR10" s="72"/>
-      <c r="AS10" s="102" t="s">
-        <v>180</v>
-      </c>
-      <c r="AT10" s="103"/>
-      <c r="AU10" s="103"/>
-      <c r="AV10" s="103"/>
-      <c r="AW10" s="103"/>
-      <c r="AX10" s="103"/>
-      <c r="AY10" s="103"/>
-      <c r="AZ10" s="103"/>
-      <c r="BA10" s="103"/>
-      <c r="BB10" s="103"/>
-      <c r="BC10" s="103"/>
-      <c r="BD10" s="103"/>
-      <c r="BE10" s="103"/>
-      <c r="BF10" s="103"/>
-      <c r="BG10" s="103"/>
-      <c r="BH10" s="103"/>
-      <c r="BI10" s="103"/>
-      <c r="BJ10" s="103"/>
-      <c r="BK10" s="103"/>
-      <c r="BL10" s="103"/>
-      <c r="BM10" s="103"/>
-      <c r="BN10" s="103"/>
-      <c r="BO10" s="103"/>
-      <c r="BP10" s="103"/>
-      <c r="BQ10" s="103"/>
-      <c r="BR10" s="103"/>
-      <c r="BS10" s="103"/>
-      <c r="BT10" s="103"/>
-      <c r="BU10" s="103"/>
-      <c r="BV10" s="103"/>
-      <c r="BW10" s="104"/>
-    </row>
-    <row r="11" spans="2:75" ht="15" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="81"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="16" t="s">
+      <c r="N10" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="68"/>
+      <c r="AD10" s="68"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="68"/>
+      <c r="AG10" s="68"/>
+      <c r="AH10" s="68"/>
+      <c r="AI10" s="68"/>
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="68"/>
+      <c r="AL10" s="68"/>
+      <c r="AM10" s="68"/>
+      <c r="AN10" s="68"/>
+      <c r="AO10" s="68"/>
+      <c r="AP10" s="68"/>
+      <c r="AQ10" s="68"/>
+      <c r="AR10" s="68"/>
+      <c r="AS10" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="AT10" s="48"/>
+      <c r="AU10" s="48"/>
+      <c r="AV10" s="48"/>
+      <c r="AW10" s="48"/>
+      <c r="AX10" s="48"/>
+      <c r="AY10" s="48"/>
+      <c r="AZ10" s="48"/>
+      <c r="BA10" s="48"/>
+      <c r="BB10" s="48"/>
+      <c r="BC10" s="48"/>
+      <c r="BD10" s="48"/>
+      <c r="BE10" s="48"/>
+      <c r="BF10" s="48"/>
+      <c r="BG10" s="48"/>
+      <c r="BH10" s="48"/>
+      <c r="BI10" s="48"/>
+      <c r="BJ10" s="48"/>
+      <c r="BK10" s="48"/>
+      <c r="BL10" s="48"/>
+      <c r="BM10" s="48"/>
+      <c r="BN10" s="48"/>
+      <c r="BO10" s="48"/>
+      <c r="BP10" s="48"/>
+      <c r="BQ10" s="48"/>
+      <c r="BR10" s="48"/>
+      <c r="BS10" s="48"/>
+      <c r="BT10" s="48"/>
+      <c r="BU10" s="48"/>
+      <c r="BV10" s="48"/>
+      <c r="BW10" s="49"/>
+    </row>
+    <row r="11" spans="2:75" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="71"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="43" t="s">
+      <c r="N11" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="71" t="s">
+      <c r="O11" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="71"/>
-      <c r="Q11" s="71"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="71"/>
-      <c r="T11" s="71"/>
-      <c r="U11" s="71"/>
-      <c r="V11" s="71" t="s">
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="W11" s="71"/>
-      <c r="X11" s="71"/>
-      <c r="Y11" s="71"/>
-      <c r="Z11" s="71"/>
-      <c r="AA11" s="71"/>
-      <c r="AB11" s="71"/>
-      <c r="AC11" s="71" t="s">
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="AD11" s="71"/>
-      <c r="AE11" s="71"/>
-      <c r="AF11" s="71"/>
-      <c r="AG11" s="71"/>
-      <c r="AH11" s="71"/>
-      <c r="AI11" s="71"/>
-      <c r="AJ11" s="71" t="s">
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
+      <c r="AH11" s="69"/>
+      <c r="AI11" s="69"/>
+      <c r="AJ11" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="AK11" s="71"/>
-      <c r="AL11" s="71"/>
-      <c r="AM11" s="71"/>
-      <c r="AN11" s="71"/>
-      <c r="AO11" s="71"/>
-      <c r="AP11" s="71"/>
-      <c r="AQ11" s="71" t="s">
-        <v>178</v>
-      </c>
-      <c r="AR11" s="71"/>
-      <c r="AS11" s="105" t="s">
+      <c r="AK11" s="69"/>
+      <c r="AL11" s="69"/>
+      <c r="AM11" s="69"/>
+      <c r="AN11" s="69"/>
+      <c r="AO11" s="69"/>
+      <c r="AP11" s="69"/>
+      <c r="AQ11" s="69" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR11" s="69"/>
+      <c r="AS11" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="AT11" s="106"/>
-      <c r="AU11" s="106"/>
-      <c r="AV11" s="106"/>
-      <c r="AW11" s="107"/>
-      <c r="AX11" s="71" t="s">
+      <c r="AT11" s="76"/>
+      <c r="AU11" s="76"/>
+      <c r="AV11" s="76"/>
+      <c r="AW11" s="77"/>
+      <c r="AX11" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AY11" s="71"/>
-      <c r="AZ11" s="71"/>
-      <c r="BA11" s="71"/>
-      <c r="BB11" s="71"/>
-      <c r="BC11" s="71"/>
-      <c r="BD11" s="71"/>
-      <c r="BE11" s="71" t="s">
+      <c r="AY11" s="69"/>
+      <c r="AZ11" s="69"/>
+      <c r="BA11" s="69"/>
+      <c r="BB11" s="69"/>
+      <c r="BC11" s="69"/>
+      <c r="BD11" s="69"/>
+      <c r="BE11" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="BF11" s="71"/>
-      <c r="BG11" s="71"/>
-      <c r="BH11" s="71"/>
-      <c r="BI11" s="71"/>
-      <c r="BJ11" s="71"/>
-      <c r="BK11" s="71"/>
-      <c r="BL11" s="71" t="s">
+      <c r="BF11" s="69"/>
+      <c r="BG11" s="69"/>
+      <c r="BH11" s="69"/>
+      <c r="BI11" s="69"/>
+      <c r="BJ11" s="69"/>
+      <c r="BK11" s="69"/>
+      <c r="BL11" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="BM11" s="71"/>
-      <c r="BN11" s="71"/>
-      <c r="BO11" s="71"/>
-      <c r="BP11" s="71"/>
-      <c r="BQ11" s="71"/>
-      <c r="BR11" s="71"/>
-      <c r="BS11" s="71" t="s">
+      <c r="BM11" s="69"/>
+      <c r="BN11" s="69"/>
+      <c r="BO11" s="69"/>
+      <c r="BP11" s="69"/>
+      <c r="BQ11" s="69"/>
+      <c r="BR11" s="69"/>
+      <c r="BS11" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="BT11" s="71"/>
-      <c r="BU11" s="71"/>
-      <c r="BV11" s="71"/>
-      <c r="BW11" s="71"/>
-    </row>
-    <row r="12" spans="2:75" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B12" s="82"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="16" t="s">
+      <c r="BT11" s="69"/>
+      <c r="BU11" s="69"/>
+      <c r="BV11" s="69"/>
+      <c r="BW11" s="69"/>
+    </row>
+    <row r="12" spans="2:75" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="115"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="N12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>17</v>
@@ -2529,13 +2626,13 @@
         <v>44</v>
       </c>
       <c r="AR12" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="AS12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="AT12" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="AU12" s="5" t="s">
         <v>17</v>
@@ -2622,280 +2719,270 @@
         <v>44</v>
       </c>
       <c r="BW12" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B13" s="75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="110" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H13" s="44">
-        <v>1</v>
-      </c>
-      <c r="I13" s="10">
-        <v>1</v>
-      </c>
-      <c r="J13" s="108">
+      <c r="F13" s="98"/>
+      <c r="G13" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="112">
+        <v>1</v>
+      </c>
+      <c r="I13" s="113">
+        <v>1</v>
+      </c>
+      <c r="J13" s="114">
         <v>45127</v>
       </c>
-      <c r="K13" s="108">
+      <c r="K13" s="114">
         <v>45127</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="19" t="s">
         <v>90</v>
       </c>
       <c r="AG13" s="6"/>
     </row>
-    <row r="14" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B14" s="77"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="36" t="s">
+    <row r="14" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H14" s="44">
-        <v>1</v>
-      </c>
-      <c r="I14" s="11">
-        <v>1</v>
-      </c>
-      <c r="J14" s="109">
+      <c r="F14" s="98"/>
+      <c r="G14" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="H14" s="119">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="45">
         <v>45128</v>
       </c>
-      <c r="K14" s="108">
+      <c r="K14" s="45">
         <v>45128</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="20" t="s">
         <v>77</v>
       </c>
       <c r="AH14" s="6"/>
     </row>
-    <row r="15" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B15" s="75" t="s">
+    <row r="15" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="84"/>
-      <c r="G15" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" s="44">
+      <c r="F15" s="98"/>
+      <c r="G15" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" s="121">
         <v>1</v>
       </c>
       <c r="I15" s="10">
         <v>2</v>
       </c>
-      <c r="J15" s="108">
+      <c r="J15" s="42">
         <v>45131</v>
       </c>
-      <c r="K15" s="108">
+      <c r="K15" s="42">
         <v>45132</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="N15" s="101"/>
-      <c r="O15" s="101"/>
-      <c r="P15" s="101"/>
+        <v>161</v>
+      </c>
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
     </row>
-    <row r="16" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B16" s="76"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="18" t="s">
+    <row r="16" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="60"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H16" s="44">
+      <c r="F16" s="98"/>
+      <c r="G16" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="40">
         <v>1</v>
       </c>
       <c r="I16" s="9">
         <v>2</v>
       </c>
-      <c r="J16" s="108">
+      <c r="J16" s="44">
         <v>45131</v>
       </c>
-      <c r="K16" s="108">
+      <c r="K16" s="44">
         <v>45132</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="N16" s="101"/>
-      <c r="O16" s="101"/>
-      <c r="P16" s="101"/>
+        <v>161</v>
+      </c>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
     </row>
-    <row r="17" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B17" s="76"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="18" t="s">
+    <row r="17" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="60"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="84"/>
-      <c r="G17" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H17" s="44">
+      <c r="F17" s="98"/>
+      <c r="G17" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="40">
         <v>1</v>
       </c>
       <c r="I17" s="9">
         <v>1</v>
       </c>
-      <c r="J17" s="108">
+      <c r="J17" s="44">
         <v>45132</v>
       </c>
-      <c r="K17" s="108">
+      <c r="K17" s="44">
         <v>45132</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="N17" s="101"/>
-      <c r="O17" s="101"/>
-      <c r="P17" s="101"/>
-      <c r="AK17" s="101"/>
+        <v>165</v>
+      </c>
       <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="76"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="18" t="s">
+    <row r="18" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="60"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H18" s="44">
+      <c r="F18" s="98"/>
+      <c r="G18" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="40">
         <v>1</v>
       </c>
       <c r="I18" s="9">
         <v>2</v>
       </c>
-      <c r="J18" s="110">
+      <c r="J18" s="44">
         <v>45133</v>
       </c>
-      <c r="K18" s="110">
+      <c r="K18" s="44">
         <v>45134</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
     </row>
-    <row r="19" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B19" s="76"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="18" t="s">
+    <row r="19" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="60"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="84"/>
-      <c r="G19" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H19" s="44">
+      <c r="F19" s="98"/>
+      <c r="G19" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="40">
         <v>1</v>
       </c>
       <c r="I19" s="9">
         <v>2</v>
       </c>
-      <c r="J19" s="110">
+      <c r="J19" s="44">
         <v>45133</v>
       </c>
-      <c r="K19" s="110">
+      <c r="K19" s="44">
         <v>45134</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AM19" s="6"/>
       <c r="AN19" s="6"/>
     </row>
-    <row r="20" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="76"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="18" t="s">
+    <row r="20" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="60"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="84"/>
-      <c r="G20" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H20" s="44">
+      <c r="F20" s="98"/>
+      <c r="G20" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="40">
         <v>1</v>
       </c>
       <c r="I20" s="9">
         <v>1</v>
       </c>
-      <c r="J20" s="110">
+      <c r="J20" s="44">
         <v>45135</v>
       </c>
-      <c r="K20" s="110">
+      <c r="K20" s="44">
         <v>45135</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B21" s="77"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="39" t="s">
+    <row r="21" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="53"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="84"/>
-      <c r="G21" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H21" s="44">
+      <c r="F21" s="98"/>
+      <c r="G21" s="108" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="122">
         <v>1</v>
       </c>
       <c r="I21" s="11">
         <v>1</v>
       </c>
-      <c r="J21" s="110">
+      <c r="J21" s="43">
         <v>45135</v>
       </c>
-      <c r="K21" s="110">
+      <c r="K21" s="43">
         <v>45135</v>
       </c>
       <c r="L21" s="14" t="s">
@@ -2903,305 +2990,305 @@
       </c>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B22" s="75" t="s">
+    <row r="22" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="85"/>
-      <c r="G22" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H22" s="44">
-        <v>1</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1</v>
-      </c>
-      <c r="J22" s="108">
+      <c r="F22" s="99"/>
+      <c r="G22" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" s="112">
+        <v>1</v>
+      </c>
+      <c r="I22" s="113">
+        <v>1</v>
+      </c>
+      <c r="J22" s="114">
         <v>45138</v>
       </c>
-      <c r="K22" s="108">
+      <c r="K22" s="114">
         <v>45138</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR22" s="6"/>
+    </row>
+    <row r="23" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="99"/>
+      <c r="G23" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" s="40">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
+      <c r="J23" s="44">
+        <v>45138</v>
+      </c>
+      <c r="K23" s="44">
+        <v>45138</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR23" s="6"/>
+    </row>
+    <row r="24" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="99"/>
+      <c r="G24" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H24" s="40">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1</v>
+      </c>
+      <c r="J24" s="44">
+        <v>45139</v>
+      </c>
+      <c r="K24" s="44">
+        <v>45139</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS24" s="6"/>
+    </row>
+    <row r="25" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="99"/>
+      <c r="G25" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" s="40">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
+      </c>
+      <c r="J25" s="44">
+        <v>45138</v>
+      </c>
+      <c r="K25" s="44">
+        <v>45138</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR25" s="6"/>
+    </row>
+    <row r="26" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="99"/>
+      <c r="G26" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H26" s="40">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1</v>
+      </c>
+      <c r="J26" s="44">
+        <v>45139</v>
+      </c>
+      <c r="K26" s="44">
+        <v>45139</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS26" s="6"/>
+    </row>
+    <row r="27" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="100"/>
+      <c r="G27" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="H27" s="119">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16">
+        <v>1</v>
+      </c>
+      <c r="J27" s="45">
+        <v>45139</v>
+      </c>
+      <c r="K27" s="45">
+        <v>45139</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS27" s="6"/>
+    </row>
+    <row r="28" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="H28" s="121">
+        <v>1</v>
+      </c>
+      <c r="I28" s="10">
+        <v>3</v>
+      </c>
+      <c r="J28" s="42">
+        <v>45140</v>
+      </c>
+      <c r="K28" s="42">
+        <v>45142</v>
+      </c>
+      <c r="L28" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="AR22" s="6"/>
-    </row>
-    <row r="23" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H23" s="44">
-        <v>1</v>
-      </c>
-      <c r="I23" s="10">
-        <v>1</v>
-      </c>
-      <c r="J23" s="108">
-        <v>45138</v>
-      </c>
-      <c r="K23" s="108">
-        <v>45138</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="AR23" s="6"/>
-    </row>
-    <row r="24" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="85"/>
-      <c r="G24" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H24" s="44">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9">
-        <v>1</v>
-      </c>
-      <c r="J24" s="110">
-        <v>45139</v>
-      </c>
-      <c r="K24" s="110">
-        <v>45139</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS24" s="6"/>
-    </row>
-    <row r="25" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="85"/>
-      <c r="G25" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H25" s="44">
-        <v>1</v>
-      </c>
-      <c r="I25" s="10">
-        <v>1</v>
-      </c>
-      <c r="J25" s="108">
-        <v>45138</v>
-      </c>
-      <c r="K25" s="108">
-        <v>45138</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="AR25" s="6"/>
-    </row>
-    <row r="26" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B26" s="76"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="85"/>
-      <c r="G26" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H26" s="44">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9">
-        <v>1</v>
-      </c>
-      <c r="J26" s="110">
-        <v>45139</v>
-      </c>
-      <c r="K26" s="110">
-        <v>45139</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS26" s="6"/>
-    </row>
-    <row r="27" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="86"/>
-      <c r="G27" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H27" s="44">
-        <v>1</v>
-      </c>
-      <c r="I27" s="9">
-        <v>1</v>
-      </c>
-      <c r="J27" s="110">
-        <v>45139</v>
-      </c>
-      <c r="K27" s="110">
-        <v>45139</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS27" s="6"/>
-    </row>
-    <row r="28" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B28" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="90" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="90" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H28" s="44">
-        <v>1</v>
-      </c>
-      <c r="I28" s="17">
-        <v>3</v>
-      </c>
-      <c r="J28" s="111">
-        <v>45140</v>
-      </c>
-      <c r="K28" s="111">
-        <v>45142</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>181</v>
       </c>
       <c r="AT28" s="6"/>
       <c r="AU28" s="6"/>
       <c r="AV28" s="6"/>
     </row>
-    <row r="29" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B29" s="76"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="36" t="s">
+    <row r="29" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="60"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="44">
-        <v>1</v>
-      </c>
-      <c r="I29" s="17">
+      <c r="G29" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H29" s="40">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
         <v>3</v>
       </c>
-      <c r="J29" s="111">
+      <c r="J29" s="44">
         <v>45140</v>
       </c>
-      <c r="K29" s="111">
+      <c r="K29" s="44">
         <v>45142</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="13" t="s">
         <v>77</v>
       </c>
       <c r="AT29" s="6"/>
       <c r="AU29" s="6"/>
       <c r="AV29" s="6"/>
     </row>
-    <row r="30" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B30" s="76"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="100" t="s">
+    <row r="30" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="60"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" s="44">
-        <v>1</v>
-      </c>
-      <c r="I30" s="17">
+      <c r="G30" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H30" s="40">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9">
         <v>3</v>
       </c>
-      <c r="J30" s="111">
+      <c r="J30" s="44">
         <v>45140</v>
       </c>
-      <c r="K30" s="111">
+      <c r="K30" s="44">
         <v>45142</v>
       </c>
-      <c r="L30" s="20" t="s">
-        <v>165</v>
+      <c r="L30" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="AT30" s="6"/>
       <c r="AU30" s="6"/>
       <c r="AV30" s="6"/>
     </row>
-    <row r="31" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B31" s="76"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="37" t="s">
+    <row r="31" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="60"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H31" s="44">
-        <v>1</v>
-      </c>
-      <c r="I31" s="17">
+      <c r="G31" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H31" s="40">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
         <v>3</v>
       </c>
-      <c r="J31" s="111">
+      <c r="J31" s="44">
         <v>45140</v>
       </c>
-      <c r="K31" s="111">
+      <c r="K31" s="44">
         <v>45142</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="O31" s="4" t="s">
         <v>117</v>
@@ -3210,714 +3297,714 @@
       <c r="AU31" s="6"/>
       <c r="AV31" s="6"/>
     </row>
-    <row r="32" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B32" s="76"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="27" t="s">
+    <row r="32" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="60"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="44">
-        <v>1</v>
-      </c>
-      <c r="I32" s="17">
+      <c r="G32" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H32" s="40">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9">
         <v>3</v>
       </c>
-      <c r="J32" s="111">
+      <c r="J32" s="44">
         <v>45140</v>
       </c>
-      <c r="K32" s="111">
+      <c r="K32" s="44">
         <v>45142</v>
       </c>
-      <c r="L32" s="14" t="s">
-        <v>165</v>
+      <c r="L32" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="AT32" s="6"/>
       <c r="AU32" s="6"/>
       <c r="AV32" s="6"/>
     </row>
-    <row r="33" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B33" s="76"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="28" t="s">
+    <row r="33" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="60"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="44">
-        <v>1</v>
-      </c>
-      <c r="I33" s="17">
+      <c r="G33" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H33" s="40">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9">
         <v>3</v>
       </c>
-      <c r="J33" s="111">
+      <c r="J33" s="44">
         <v>45140</v>
       </c>
-      <c r="K33" s="111">
+      <c r="K33" s="44">
         <v>45142</v>
       </c>
-      <c r="L33" s="12" t="s">
-        <v>165</v>
+      <c r="L33" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="AT33" s="6"/>
       <c r="AU33" s="6"/>
       <c r="AV33" s="6"/>
     </row>
-    <row r="34" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B34" s="76"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="73" t="s">
+    <row r="34" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="60"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G34" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="44">
-        <v>1</v>
-      </c>
-      <c r="I34" s="17">
+      <c r="G34" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="40">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9">
         <v>3</v>
       </c>
-      <c r="J34" s="111">
+      <c r="J34" s="44">
         <v>45140</v>
       </c>
-      <c r="K34" s="111">
+      <c r="K34" s="44">
         <v>45142</v>
       </c>
-      <c r="L34" s="21" t="s">
+      <c r="L34" s="13" t="s">
         <v>77</v>
       </c>
       <c r="AT34" s="6"/>
       <c r="AU34" s="6"/>
       <c r="AV34" s="6"/>
     </row>
-    <row r="35" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B35" s="76"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="32" t="s">
+    <row r="35" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="60"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" s="44">
-        <v>1</v>
-      </c>
-      <c r="I35" s="17">
+      <c r="G35" s="108" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" s="122">
+        <v>1</v>
+      </c>
+      <c r="I35" s="11">
         <v>3</v>
       </c>
-      <c r="J35" s="111">
+      <c r="J35" s="43">
         <v>45140</v>
       </c>
-      <c r="K35" s="111">
+      <c r="K35" s="43">
         <v>45142</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L35" s="14" t="s">
         <v>77</v>
       </c>
       <c r="AT35" s="6"/>
       <c r="AU35" s="6"/>
       <c r="AV35" s="6"/>
     </row>
-    <row r="36" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B36" s="57" t="s">
+    <row r="36" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="33" t="s">
+      <c r="F36" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G36" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="44">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7">
-        <v>1</v>
-      </c>
-      <c r="J36" s="112">
+      <c r="G36" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="H36" s="112">
+        <v>1</v>
+      </c>
+      <c r="I36" s="123">
+        <v>1</v>
+      </c>
+      <c r="J36" s="124">
         <v>45145</v>
       </c>
-      <c r="K36" s="112">
+      <c r="K36" s="124">
         <v>45145</v>
       </c>
-      <c r="L36" s="13" t="s">
-        <v>169</v>
+      <c r="L36" s="19" t="s">
+        <v>161</v>
       </c>
       <c r="AW36" s="6"/>
     </row>
-    <row r="37" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="73" t="s">
+    <row r="37" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="44">
+      <c r="G37" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H37" s="40">
         <v>1</v>
       </c>
       <c r="I37" s="7">
         <v>1</v>
       </c>
-      <c r="J37" s="112">
+      <c r="J37" s="46">
         <v>45145</v>
       </c>
-      <c r="K37" s="112">
+      <c r="K37" s="46">
         <v>45145</v>
       </c>
-      <c r="L37" s="21" t="s">
-        <v>169</v>
+      <c r="L37" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="AW37" s="6"/>
     </row>
-    <row r="38" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="28" t="s">
+    <row r="38" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H38" s="44">
-        <v>1</v>
-      </c>
-      <c r="I38" s="7">
-        <v>1</v>
-      </c>
-      <c r="J38" s="112">
+      <c r="G38" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="H38" s="119">
+        <v>1</v>
+      </c>
+      <c r="I38" s="125">
+        <v>1</v>
+      </c>
+      <c r="J38" s="126">
         <v>45145</v>
       </c>
-      <c r="K38" s="112">
+      <c r="K38" s="126">
         <v>45145</v>
       </c>
-      <c r="L38" s="21" t="s">
-        <v>169</v>
+      <c r="L38" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="AW38" s="6"/>
     </row>
-    <row r="39" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="73" t="s">
+    <row r="39" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="44">
-        <v>1</v>
-      </c>
-      <c r="I39" s="7">
-        <v>1</v>
-      </c>
-      <c r="J39" s="112">
+      <c r="G39" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="H39" s="121">
+        <v>1</v>
+      </c>
+      <c r="I39" s="127">
+        <v>1</v>
+      </c>
+      <c r="J39" s="128">
         <v>45145</v>
       </c>
-      <c r="K39" s="112">
+      <c r="K39" s="128">
         <v>45145</v>
       </c>
-      <c r="L39" s="21" t="s">
-        <v>169</v>
+      <c r="L39" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="AW39" s="6"/>
     </row>
-    <row r="40" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="22" t="s">
+    <row r="40" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H40" s="44">
-        <v>1</v>
-      </c>
-      <c r="I40" s="7">
-        <v>1</v>
-      </c>
-      <c r="J40" s="112">
+      <c r="G40" s="108" t="s">
+        <v>167</v>
+      </c>
+      <c r="H40" s="122">
+        <v>1</v>
+      </c>
+      <c r="I40" s="109">
+        <v>1</v>
+      </c>
+      <c r="J40" s="129">
         <v>45145</v>
       </c>
-      <c r="K40" s="112">
+      <c r="K40" s="129">
         <v>45145</v>
       </c>
-      <c r="L40" s="21" t="s">
-        <v>169</v>
+      <c r="L40" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="AW40" s="6"/>
     </row>
-    <row r="41" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="73" t="s">
+    <row r="41" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F41" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" s="44">
-        <v>1</v>
-      </c>
-      <c r="I41" s="7">
-        <v>1</v>
-      </c>
-      <c r="J41" s="112">
+      <c r="G41" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="H41" s="112">
+        <v>1</v>
+      </c>
+      <c r="I41" s="123">
+        <v>1</v>
+      </c>
+      <c r="J41" s="124">
         <v>45145</v>
       </c>
-      <c r="K41" s="112">
+      <c r="K41" s="124">
         <v>45145</v>
       </c>
-      <c r="L41" s="21" t="s">
-        <v>169</v>
+      <c r="L41" s="19" t="s">
+        <v>161</v>
       </c>
       <c r="AW41" s="6"/>
     </row>
-    <row r="42" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="74"/>
+    <row r="42" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="67"/>
       <c r="F42" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="113" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="44">
-        <v>1</v>
-      </c>
-      <c r="I42" s="7">
-        <v>1</v>
-      </c>
-      <c r="J42" s="112">
+      <c r="G42" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="H42" s="119">
+        <v>1</v>
+      </c>
+      <c r="I42" s="125">
+        <v>1</v>
+      </c>
+      <c r="J42" s="126">
         <v>45145</v>
       </c>
-      <c r="K42" s="112">
+      <c r="K42" s="126">
         <v>45145</v>
       </c>
-      <c r="L42" s="21" t="s">
-        <v>169</v>
+      <c r="L42" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="AW42" s="6"/>
     </row>
-    <row r="43" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="60" t="s">
+    <row r="43" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="65"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="63" t="s">
+      <c r="E43" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I43" s="127"/>
+      <c r="J43" s="127"/>
+      <c r="K43" s="127"/>
+      <c r="L43" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="F43" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="G43" s="9" t="s">
+      <c r="G44" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H43" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="G45" s="9" t="s">
+      <c r="L44" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="101" t="s">
+        <v>132</v>
+      </c>
+      <c r="G45" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="7" t="s">
+      <c r="L45" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="G46" s="9" t="s">
+    <row r="46" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="101" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="47" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="G47" s="9" t="s">
+      <c r="L46" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="G47" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="G48" s="9" t="s">
+      <c r="L47" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="102" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="40" t="s">
+      <c r="I48" s="109"/>
+      <c r="J48" s="109"/>
+      <c r="K48" s="109"/>
+      <c r="L48" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="38" t="s">
         <v>120</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="G49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G49" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="H49" s="17" t="s">
+      <c r="H49" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="48" t="s">
+      <c r="I49" s="132"/>
+      <c r="J49" s="132"/>
+      <c r="K49" s="132"/>
+      <c r="L49" s="133" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="G50" s="9" t="s">
+      <c r="F50" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="H50" s="17" t="s">
+      <c r="H50" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="G51" s="9" t="s">
+      <c r="I50" s="127"/>
+      <c r="J50" s="127"/>
+      <c r="K50" s="127"/>
+      <c r="L50" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="65"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="H51" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
-      <c r="L51" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="25" t="s">
+      <c r="L51" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="H52" s="17" t="s">
+      <c r="H52" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-    </row>
-    <row r="54" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>98</v>
+      <c r="I52" s="125"/>
+      <c r="J52" s="125"/>
+      <c r="K52" s="125"/>
+      <c r="L52" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="82" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="121">
+        <v>1</v>
+      </c>
+      <c r="I53" s="127"/>
+      <c r="J53" s="127"/>
+      <c r="K53" s="127"/>
+      <c r="L53" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="134"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="G54" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="H54" s="40">
+        <v>1</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-    </row>
-    <row r="55" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="G55" s="9" t="s">
+      <c r="L54" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="134"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="G55" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="H55" s="17" t="s">
-        <v>98</v>
+      <c r="H55" s="40">
+        <v>1</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="7" t="s">
+      <c r="L55" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="134"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="G56" s="118" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="119">
+        <v>1</v>
+      </c>
+      <c r="I56" s="125"/>
+      <c r="J56" s="125"/>
+      <c r="K56" s="125"/>
+      <c r="L56" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="F57" s="103" t="s">
+        <v>177</v>
+      </c>
+      <c r="G57" s="120" t="s">
+        <v>72</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I57" s="127"/>
+      <c r="J57" s="127"/>
+      <c r="K57" s="127"/>
+      <c r="L57" s="12"/>
+    </row>
+    <row r="58" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B58" s="65"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="87"/>
+      <c r="F58" s="102" t="s">
+        <v>178</v>
+      </c>
+      <c r="G58" s="108" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I58" s="109"/>
+      <c r="J58" s="109"/>
+      <c r="K58" s="109"/>
+      <c r="L58" s="14"/>
+    </row>
+    <row r="59" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="65"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="F59" s="103" t="s">
+        <v>179</v>
+      </c>
+      <c r="G59" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="H59" s="113" t="s">
+        <v>98</v>
+      </c>
+      <c r="I59" s="123"/>
+      <c r="J59" s="123"/>
+      <c r="K59" s="123"/>
+      <c r="L59" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B56" s="58"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H57" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="62"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="E59" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="F59" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-    </row>
-    <row r="60" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="G60" s="9" t="s">
+    <row r="60" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="65"/>
+      <c r="C60" s="65"/>
+      <c r="D60" s="95"/>
+      <c r="E60" s="86"/>
+      <c r="F60" s="101" t="s">
+        <v>180</v>
+      </c>
+      <c r="G60" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H60" s="9" t="s">
@@ -3926,19 +4013,19 @@
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
-      <c r="L60" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="G61" s="9" t="s">
+      <c r="L60" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="65"/>
+      <c r="C61" s="65"/>
+      <c r="D61" s="95"/>
+      <c r="E61" s="86"/>
+      <c r="F61" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="G61" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H61" s="9" t="s">
@@ -3947,61 +4034,63 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="G62" s="9" t="s">
+      <c r="L61" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B62" s="65"/>
+      <c r="C62" s="65"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="87"/>
+      <c r="F62" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="G62" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="H62" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7" t="s">
+      <c r="I62" s="109"/>
+      <c r="J62" s="109"/>
+      <c r="K62" s="109"/>
+      <c r="L62" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="G63" s="9" t="s">
+    <row r="63" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="65"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="G63" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="H63" s="9" t="s">
+      <c r="H63" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="55"/>
-      <c r="E64" s="52"/>
-      <c r="F64" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="G64" s="9" t="s">
+      <c r="I63" s="123"/>
+      <c r="J63" s="123"/>
+      <c r="K63" s="123"/>
+      <c r="L63" s="19"/>
+    </row>
+    <row r="64" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="65"/>
+      <c r="C64" s="65"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="101" t="s">
+        <v>136</v>
+      </c>
+      <c r="G64" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H64" s="9" t="s">
@@ -4010,19 +4099,19 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="G65" s="9" t="s">
+      <c r="L64" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="65"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="89"/>
+      <c r="F65" s="101" t="s">
+        <v>137</v>
+      </c>
+      <c r="G65" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H65" s="9" t="s">
@@ -4031,21 +4120,19 @@
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
-      <c r="L65" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B66" s="58"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="G66" s="9" t="s">
+      <c r="L65" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="65"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="92"/>
+      <c r="E66" s="89"/>
+      <c r="F66" s="101" t="s">
+        <v>138</v>
+      </c>
+      <c r="G66" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H66" s="9" t="s">
@@ -4054,19 +4141,19 @@
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
-      <c r="L66" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B67" s="58"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="55"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G67" s="9" t="s">
+      <c r="L66" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="65"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="89"/>
+      <c r="F67" s="101" t="s">
+        <v>139</v>
+      </c>
+      <c r="G67" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H67" s="9" t="s">
@@ -4075,21 +4162,19 @@
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
-      <c r="L67" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B68" s="59"/>
-      <c r="C68" s="59"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="F68" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="G68" s="9" t="s">
+      <c r="L67" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="65"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="89"/>
+      <c r="F68" s="101" t="s">
+        <v>140</v>
+      </c>
+      <c r="G68" s="107" t="s">
         <v>49</v>
       </c>
       <c r="H68" s="9" t="s">
@@ -4098,74 +4183,64 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
-      <c r="L68" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B69" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C69" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="H69" s="9" t="s">
+      <c r="L68" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B69" s="65"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="90"/>
+      <c r="F69" s="104" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="118" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="G70" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="H70" s="9" t="s">
+      <c r="I69" s="125"/>
+      <c r="J69" s="125"/>
+      <c r="K69" s="125"/>
+      <c r="L69" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="65"/>
+      <c r="C70" s="65"/>
+      <c r="D70" s="92"/>
+      <c r="E70" s="85" t="s">
+        <v>142</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G70" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H70" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="49"/>
-      <c r="E71" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>71</v>
+      <c r="I70" s="127"/>
+      <c r="J70" s="127"/>
+      <c r="K70" s="127"/>
+      <c r="L70" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
+      <c r="D71" s="92"/>
+      <c r="E71" s="87"/>
+      <c r="F71" s="101" t="s">
+        <v>144</v>
+      </c>
+      <c r="G71" s="107" t="s">
+        <v>49</v>
       </c>
       <c r="H71" s="9" t="s">
         <v>98</v>
@@ -4173,48 +4248,164 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
-      <c r="L71" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="25" t="s">
+      <c r="L71" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="93"/>
+      <c r="E72" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="F72" s="104" t="s">
+        <v>146</v>
+      </c>
+      <c r="G72" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I72" s="109"/>
+      <c r="J72" s="109"/>
+      <c r="K72" s="109"/>
+      <c r="L72" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="F72" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G72" s="15" t="s">
+    </row>
+    <row r="73" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B73" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="82" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="85" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G73" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H73" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7" t="s">
-        <v>169</v>
+      <c r="I73" s="123"/>
+      <c r="J73" s="123"/>
+      <c r="K73" s="123"/>
+      <c r="L73" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B74" s="83"/>
+      <c r="C74" s="83"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F74" s="101" t="s">
+        <v>152</v>
+      </c>
+      <c r="G74" s="107" t="s">
+        <v>71</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B75" s="83"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="86"/>
+      <c r="E75" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F75" s="101" t="s">
+        <v>154</v>
+      </c>
+      <c r="G75" s="107" t="s">
+        <v>71</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B76" s="84"/>
+      <c r="C76" s="84"/>
+      <c r="D76" s="87"/>
+      <c r="E76" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F76" s="102" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="108" t="s">
+        <v>71</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I76" s="109"/>
+      <c r="J76" s="109"/>
+      <c r="K76" s="109"/>
+      <c r="L76" s="14" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="AS10:BW10"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="D28:D35"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="D15:D21"/>
+  <mergeCells count="63">
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="D73:D76"/>
+    <mergeCell ref="E63:E69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="D63:D72"/>
+    <mergeCell ref="C36:C72"/>
+    <mergeCell ref="B36:B72"/>
+    <mergeCell ref="D43:D62"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="BL11:BR11"/>
+    <mergeCell ref="AJ11:AP11"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="AS11:AW11"/>
+    <mergeCell ref="I10:I12"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="B15:B21"/>
     <mergeCell ref="C15:C21"/>
@@ -4229,41 +4420,24 @@
     <mergeCell ref="F13:F27"/>
     <mergeCell ref="D36:D42"/>
     <mergeCell ref="B28:B35"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="AS10:BW10"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="D28:D35"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="D15:D21"/>
     <mergeCell ref="BS11:BW11"/>
     <mergeCell ref="AX11:BD11"/>
     <mergeCell ref="BE11:BK11"/>
-    <mergeCell ref="BL11:BR11"/>
-    <mergeCell ref="AJ11:AP11"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="AS11:AW11"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="E59:E65"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="D59:D68"/>
-    <mergeCell ref="C36:C68"/>
-    <mergeCell ref="B36:B68"/>
-    <mergeCell ref="D43:D58"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E39:E40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Header CSS 변경 및 WBS 수정
</commit_message>
<xml_diff>
--- a/WBS_Pro01_작업자,일정 표시 필요.xlsx
+++ b/WBS_Pro01_작업자,일정 표시 필요.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlsdp\Desktop\github\Chunjae_Team_Proj01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFDBA7F-7C81-4E67-AE75-FE808212B220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
   <si>
     <t>프로젝트 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -565,192 +559,220 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>2. 권한 기능 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 관리자 공지사항, 커뮤니티, Q&amp;A, FAQ 게시판 권한 기능 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 회원 전용 Q&amp;A, 커뮤니티 게시판 제한적 권한 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 댓글 기능 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 커뮤니티, Q&amp;A 댓글 기능 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 및 환경 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 개발 환경 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 각 개인의 컴퓨터 혹은 학과 내 실습실 컴퓨터로 구동 가능 여부 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 단위 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 기능 별 단위테스트 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 통합테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1 통합테스트 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 최종 검수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1 최종 검수 및 수정사항 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김현경, 김보경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김보경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신예은, 박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김현경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전 원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오태훈, 박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김보경, 신예은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김현경, 박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ver.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>31D</t>
+  </si>
+  <si>
+    <t>6W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신예은, 김보경, 김현경, 박진권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 관리자 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 소개 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 게시판 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1 회사 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2 서비스 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.1 학부모 커뮤니티 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2 Q&amp;A 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.3 FAQ 게시판 HTML5+CSS3 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.4 공지사항 게시판 HTML5+CSS3 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-1. 관리자 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2. 회원관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-3. 고객지원 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-4. 게시판 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-2. 관리자 개인 정보 변경 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신예은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.7 공지사항 게시판 JSP 스크립트릿 언어 작성 및 SQL DB 연결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2. 권한 기능 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1 관리자 공지사항, 커뮤니티, Q&amp;A, FAQ 게시판 권한 기능 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2 회원 전용 Q&amp;A, 커뮤니티 게시판 제한적 권한 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. 댓글 기능 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. 커뮤니티, Q&amp;A 댓글 기능 부여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능 및 환경 테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 개발 환경 테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1 각 개인의 컴퓨터 혹은 학과 내 실습실 컴퓨터로 구동 가능 여부 테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 단위 테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1 기능 별 단위테스트 진행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. 통합테스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1 통합테스트 진행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. 최종 검수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1 최종 검수 및 수정사항 진행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김현경, 김보경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김보경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신예은, 박진권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김현경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전 원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박진권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오태훈, 박진권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김보경, 신예은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김현경, 박진권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ver.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>진행완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2D</t>
-  </si>
-  <si>
-    <t>31D</t>
-  </si>
-  <si>
-    <t>6W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신예은, 김보경, 김현경, 박진권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. 관리자 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. 소개 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6. 게시판 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1 회사 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.2 서비스 소개 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.1 학부모 커뮤니티 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.2 Q&amp;A 게시판 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.3 FAQ 게시판 HTML5+CSS3 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.4 공지사항 게시판 HTML5+CSS3 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-1. 관리자 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-2. 회원관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-3. 고객지원 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4-4. 게시판 관리 페이지 HTML5+CSS3 JSP 스크립트 작업</t>
+    <t>1.8 관리자 페이지 JSP 스크립트릿 언어 작성 및 SQL DB 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오태훈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신예은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추후 작성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
@@ -864,7 +886,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1501,13 +1523,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1649,6 +1684,231 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1658,16 +1918,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1688,9 +1942,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1700,217 +1951,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2219,319 +2263,323 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:BW76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:BW78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.58203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="57.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="32.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.875" style="4" customWidth="1"/>
     <col min="7" max="10" width="8.75" style="4"/>
-    <col min="11" max="11" width="18.08203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.75" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="71" width="4.75" style="4" customWidth="1"/>
     <col min="72" max="75" width="4.75" style="1" customWidth="1"/>
     <col min="76" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="80"/>
+      <c r="E2" s="82"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="80"/>
+      <c r="E3" s="82"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="82"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="80"/>
+      <c r="E5" s="82"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="80"/>
-    </row>
-    <row r="7" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E6" s="82"/>
+    </row>
+    <row r="7" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" s="80"/>
+      <c r="D7" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="82"/>
     </row>
     <row r="9" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="2:75" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="70" t="s">
+    <row r="10" spans="2:75" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="78" t="s">
+      <c r="F10" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="78" t="s">
+      <c r="I10" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="78" t="s">
+      <c r="K10" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="105" t="s">
+      <c r="L10" s="110" t="s">
         <v>50</v>
       </c>
       <c r="M10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="68" t="s">
+      <c r="N10" s="109" t="s">
+        <v>170</v>
+      </c>
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="109"/>
+      <c r="X10" s="109"/>
+      <c r="Y10" s="109"/>
+      <c r="Z10" s="109"/>
+      <c r="AA10" s="109"/>
+      <c r="AB10" s="109"/>
+      <c r="AC10" s="109"/>
+      <c r="AD10" s="109"/>
+      <c r="AE10" s="109"/>
+      <c r="AF10" s="109"/>
+      <c r="AG10" s="109"/>
+      <c r="AH10" s="109"/>
+      <c r="AI10" s="109"/>
+      <c r="AJ10" s="109"/>
+      <c r="AK10" s="109"/>
+      <c r="AL10" s="109"/>
+      <c r="AM10" s="109"/>
+      <c r="AN10" s="109"/>
+      <c r="AO10" s="109"/>
+      <c r="AP10" s="109"/>
+      <c r="AQ10" s="109"/>
+      <c r="AR10" s="109"/>
+      <c r="AS10" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="68"/>
-      <c r="T10" s="68"/>
-      <c r="U10" s="68"/>
-      <c r="V10" s="68"/>
-      <c r="W10" s="68"/>
-      <c r="X10" s="68"/>
-      <c r="Y10" s="68"/>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="68"/>
-      <c r="AC10" s="68"/>
-      <c r="AD10" s="68"/>
-      <c r="AE10" s="68"/>
-      <c r="AF10" s="68"/>
-      <c r="AG10" s="68"/>
-      <c r="AH10" s="68"/>
-      <c r="AI10" s="68"/>
-      <c r="AJ10" s="68"/>
-      <c r="AK10" s="68"/>
-      <c r="AL10" s="68"/>
-      <c r="AM10" s="68"/>
-      <c r="AN10" s="68"/>
-      <c r="AO10" s="68"/>
-      <c r="AP10" s="68"/>
-      <c r="AQ10" s="68"/>
-      <c r="AR10" s="68"/>
-      <c r="AS10" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="AT10" s="48"/>
-      <c r="AU10" s="48"/>
-      <c r="AV10" s="48"/>
-      <c r="AW10" s="48"/>
-      <c r="AX10" s="48"/>
-      <c r="AY10" s="48"/>
-      <c r="AZ10" s="48"/>
-      <c r="BA10" s="48"/>
-      <c r="BB10" s="48"/>
-      <c r="BC10" s="48"/>
-      <c r="BD10" s="48"/>
-      <c r="BE10" s="48"/>
-      <c r="BF10" s="48"/>
-      <c r="BG10" s="48"/>
-      <c r="BH10" s="48"/>
-      <c r="BI10" s="48"/>
-      <c r="BJ10" s="48"/>
-      <c r="BK10" s="48"/>
-      <c r="BL10" s="48"/>
-      <c r="BM10" s="48"/>
-      <c r="BN10" s="48"/>
-      <c r="BO10" s="48"/>
-      <c r="BP10" s="48"/>
-      <c r="BQ10" s="48"/>
-      <c r="BR10" s="48"/>
-      <c r="BS10" s="48"/>
-      <c r="BT10" s="48"/>
-      <c r="BU10" s="48"/>
-      <c r="BV10" s="48"/>
-      <c r="BW10" s="49"/>
-    </row>
-    <row r="11" spans="2:75" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="71"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="106"/>
+      <c r="AT10" s="123"/>
+      <c r="AU10" s="123"/>
+      <c r="AV10" s="123"/>
+      <c r="AW10" s="123"/>
+      <c r="AX10" s="123"/>
+      <c r="AY10" s="123"/>
+      <c r="AZ10" s="123"/>
+      <c r="BA10" s="123"/>
+      <c r="BB10" s="123"/>
+      <c r="BC10" s="123"/>
+      <c r="BD10" s="123"/>
+      <c r="BE10" s="123"/>
+      <c r="BF10" s="123"/>
+      <c r="BG10" s="123"/>
+      <c r="BH10" s="123"/>
+      <c r="BI10" s="123"/>
+      <c r="BJ10" s="123"/>
+      <c r="BK10" s="123"/>
+      <c r="BL10" s="123"/>
+      <c r="BM10" s="123"/>
+      <c r="BN10" s="123"/>
+      <c r="BO10" s="123"/>
+      <c r="BP10" s="123"/>
+      <c r="BQ10" s="123"/>
+      <c r="BR10" s="123"/>
+      <c r="BS10" s="123"/>
+      <c r="BT10" s="123"/>
+      <c r="BU10" s="123"/>
+      <c r="BV10" s="123"/>
+      <c r="BW10" s="124"/>
+    </row>
+    <row r="11" spans="2:75" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="114"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="111"/>
       <c r="M11" s="15" t="s">
         <v>13</v>
       </c>
       <c r="N11" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="69" t="s">
+      <c r="O11" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69" t="s">
+      <c r="P11" s="101"/>
+      <c r="Q11" s="101"/>
+      <c r="R11" s="101"/>
+      <c r="S11" s="101"/>
+      <c r="T11" s="101"/>
+      <c r="U11" s="101"/>
+      <c r="V11" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="W11" s="69"/>
-      <c r="X11" s="69"/>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69" t="s">
+      <c r="W11" s="101"/>
+      <c r="X11" s="101"/>
+      <c r="Y11" s="101"/>
+      <c r="Z11" s="101"/>
+      <c r="AA11" s="101"/>
+      <c r="AB11" s="101"/>
+      <c r="AC11" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
-      <c r="AH11" s="69"/>
-      <c r="AI11" s="69"/>
-      <c r="AJ11" s="69" t="s">
+      <c r="AD11" s="101"/>
+      <c r="AE11" s="101"/>
+      <c r="AF11" s="101"/>
+      <c r="AG11" s="101"/>
+      <c r="AH11" s="101"/>
+      <c r="AI11" s="101"/>
+      <c r="AJ11" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="AK11" s="69"/>
-      <c r="AL11" s="69"/>
-      <c r="AM11" s="69"/>
-      <c r="AN11" s="69"/>
-      <c r="AO11" s="69"/>
-      <c r="AP11" s="69"/>
-      <c r="AQ11" s="69" t="s">
-        <v>170</v>
-      </c>
-      <c r="AR11" s="69"/>
-      <c r="AS11" s="75" t="s">
+      <c r="AK11" s="101"/>
+      <c r="AL11" s="101"/>
+      <c r="AM11" s="101"/>
+      <c r="AN11" s="101"/>
+      <c r="AO11" s="101"/>
+      <c r="AP11" s="101"/>
+      <c r="AQ11" s="101" t="s">
+        <v>169</v>
+      </c>
+      <c r="AR11" s="101"/>
+      <c r="AS11" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="AT11" s="76"/>
-      <c r="AU11" s="76"/>
-      <c r="AV11" s="76"/>
-      <c r="AW11" s="77"/>
-      <c r="AX11" s="69" t="s">
+      <c r="AT11" s="103"/>
+      <c r="AU11" s="103"/>
+      <c r="AV11" s="103"/>
+      <c r="AW11" s="104"/>
+      <c r="AX11" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="AY11" s="69"/>
-      <c r="AZ11" s="69"/>
-      <c r="BA11" s="69"/>
-      <c r="BB11" s="69"/>
-      <c r="BC11" s="69"/>
-      <c r="BD11" s="69"/>
-      <c r="BE11" s="69" t="s">
+      <c r="AY11" s="101"/>
+      <c r="AZ11" s="101"/>
+      <c r="BA11" s="101"/>
+      <c r="BB11" s="101"/>
+      <c r="BC11" s="101"/>
+      <c r="BD11" s="101"/>
+      <c r="BE11" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="BF11" s="69"/>
-      <c r="BG11" s="69"/>
-      <c r="BH11" s="69"/>
-      <c r="BI11" s="69"/>
-      <c r="BJ11" s="69"/>
-      <c r="BK11" s="69"/>
-      <c r="BL11" s="69" t="s">
+      <c r="BF11" s="101"/>
+      <c r="BG11" s="101"/>
+      <c r="BH11" s="101"/>
+      <c r="BI11" s="101"/>
+      <c r="BJ11" s="101"/>
+      <c r="BK11" s="101"/>
+      <c r="BL11" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="BM11" s="69"/>
-      <c r="BN11" s="69"/>
-      <c r="BO11" s="69"/>
-      <c r="BP11" s="69"/>
-      <c r="BQ11" s="69"/>
-      <c r="BR11" s="69"/>
-      <c r="BS11" s="69" t="s">
+      <c r="BM11" s="101"/>
+      <c r="BN11" s="101"/>
+      <c r="BO11" s="101"/>
+      <c r="BP11" s="101"/>
+      <c r="BQ11" s="101"/>
+      <c r="BR11" s="101"/>
+      <c r="BS11" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="BT11" s="69"/>
-      <c r="BU11" s="69"/>
-      <c r="BV11" s="69"/>
-      <c r="BW11" s="69"/>
-    </row>
-    <row r="12" spans="2:75" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="BT11" s="101"/>
+      <c r="BU11" s="101"/>
+      <c r="BV11" s="101"/>
+      <c r="BW11" s="101"/>
+    </row>
+    <row r="12" spans="2:75" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="115"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="117"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="112"/>
       <c r="M12" s="15" t="s">
         <v>14</v>
       </c>
@@ -2539,7 +2587,7 @@
         <v>16</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>17</v>
@@ -2626,13 +2674,13 @@
         <v>44</v>
       </c>
       <c r="AR12" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AS12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="AT12" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AU12" s="5" t="s">
         <v>17</v>
@@ -2719,36 +2767,37 @@
         <v>44</v>
       </c>
       <c r="BW12" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="110" t="s">
+      <c r="D13" s="126" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="98"/>
-      <c r="G13" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="H13" s="112">
-        <v>1</v>
-      </c>
-      <c r="I13" s="113">
-        <v>1</v>
-      </c>
-      <c r="J13" s="114">
+      <c r="F13" s="116"/>
+      <c r="G13" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="56">
+        <v>1</v>
+      </c>
+      <c r="I13" s="57">
+        <f t="shared" ref="I13:I52" si="0">K13-J13+1</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="58">
         <v>45127</v>
       </c>
-      <c r="K13" s="114">
+      <c r="K13" s="58">
         <v>45127</v>
       </c>
       <c r="L13" s="19" t="s">
@@ -2756,21 +2805,22 @@
       </c>
       <c r="AG13" s="6"/>
     </row>
-    <row r="14" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+    <row r="14" spans="2:75" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="108"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
       <c r="E14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="98"/>
-      <c r="G14" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="H14" s="119">
+      <c r="F14" s="116"/>
+      <c r="G14" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="60">
         <v>1</v>
       </c>
       <c r="I14" s="16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J14" s="45">
@@ -2784,27 +2834,28 @@
       </c>
       <c r="AH14" s="6"/>
     </row>
-    <row r="15" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="52" t="s">
+    <row r="15" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="92" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="98"/>
-      <c r="G15" s="120" t="s">
-        <v>167</v>
-      </c>
-      <c r="H15" s="121">
+      <c r="F15" s="116"/>
+      <c r="G15" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="62">
         <v>1</v>
       </c>
       <c r="I15" s="10">
+        <f>K15-J15+1</f>
         <v>2</v>
       </c>
       <c r="J15" s="42">
@@ -2814,26 +2865,27 @@
         <v>45132</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
     </row>
-    <row r="16" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="60"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
+    <row r="16" spans="2:75" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="107"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="98"/>
-      <c r="G16" s="107" t="s">
-        <v>167</v>
+      <c r="F16" s="116"/>
+      <c r="G16" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H16" s="40">
         <v>1</v>
       </c>
       <c r="I16" s="9">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J16" s="44">
@@ -2843,26 +2895,27 @@
         <v>45132</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
     </row>
-    <row r="17" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="60"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
+    <row r="17" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="107"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
       <c r="E17" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="98"/>
-      <c r="G17" s="107" t="s">
-        <v>167</v>
+      <c r="F17" s="116"/>
+      <c r="G17" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H17" s="40">
         <v>1</v>
       </c>
       <c r="I17" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J17" s="44">
@@ -2872,25 +2925,26 @@
         <v>45132</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="60"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
+    <row r="18" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="107"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
       <c r="E18" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="98"/>
-      <c r="G18" s="107" t="s">
-        <v>167</v>
+      <c r="F18" s="116"/>
+      <c r="G18" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H18" s="40">
         <v>1</v>
       </c>
       <c r="I18" s="9">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J18" s="44">
@@ -2900,26 +2954,27 @@
         <v>45134</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
     </row>
-    <row r="19" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="60"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
+    <row r="19" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="107"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
       <c r="E19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="107" t="s">
-        <v>167</v>
+      <c r="F19" s="116"/>
+      <c r="G19" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H19" s="40">
         <v>1</v>
       </c>
       <c r="I19" s="9">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J19" s="44">
@@ -2929,26 +2984,27 @@
         <v>45134</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AM19" s="6"/>
       <c r="AN19" s="6"/>
     </row>
-    <row r="20" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="60"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
+    <row r="20" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="107"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
       <c r="E20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="98"/>
-      <c r="G20" s="107" t="s">
-        <v>167</v>
+      <c r="F20" s="116"/>
+      <c r="G20" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H20" s="40">
         <v>1</v>
       </c>
       <c r="I20" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J20" s="44">
@@ -2958,25 +3014,26 @@
         <v>45135</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AO20" s="6"/>
     </row>
-    <row r="21" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="53"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
+    <row r="21" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="108"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
       <c r="E21" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="H21" s="122">
+      <c r="F21" s="116"/>
+      <c r="G21" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="H21" s="63">
         <v>1</v>
       </c>
       <c r="I21" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J21" s="43">
@@ -2990,55 +3047,57 @@
       </c>
       <c r="AO21" s="6"/>
     </row>
-    <row r="22" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="52" t="s">
+    <row r="22" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="133" t="s">
         <v>75</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="99"/>
-      <c r="G22" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="H22" s="112">
-        <v>1</v>
-      </c>
-      <c r="I22" s="113">
-        <v>1</v>
-      </c>
-      <c r="J22" s="114">
+      <c r="F22" s="117"/>
+      <c r="G22" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="H22" s="56">
+        <v>1</v>
+      </c>
+      <c r="I22" s="57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="58">
         <v>45138</v>
       </c>
-      <c r="K22" s="114">
+      <c r="K22" s="58">
         <v>45138</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AR22" s="6"/>
     </row>
-    <row r="23" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="62"/>
+    <row r="23" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="134"/>
       <c r="E23" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="99"/>
-      <c r="G23" s="107" t="s">
-        <v>167</v>
+      <c r="F23" s="117"/>
+      <c r="G23" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H23" s="40">
         <v>1</v>
       </c>
       <c r="I23" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J23" s="44">
@@ -3048,25 +3107,26 @@
         <v>45138</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AR23" s="6"/>
     </row>
-    <row r="24" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="62"/>
+    <row r="24" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="134"/>
       <c r="E24" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="99"/>
-      <c r="G24" s="107" t="s">
-        <v>167</v>
+      <c r="F24" s="117"/>
+      <c r="G24" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H24" s="40">
         <v>1</v>
       </c>
       <c r="I24" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J24" s="44">
@@ -3076,25 +3136,26 @@
         <v>45139</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS24" s="6"/>
     </row>
-    <row r="25" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="62"/>
+    <row r="25" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="134"/>
       <c r="E25" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="99"/>
-      <c r="G25" s="107" t="s">
-        <v>167</v>
+      <c r="F25" s="117"/>
+      <c r="G25" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H25" s="40">
         <v>1</v>
       </c>
       <c r="I25" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J25" s="44">
@@ -3104,25 +3165,26 @@
         <v>45138</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AR25" s="6"/>
     </row>
-    <row r="26" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="62"/>
+    <row r="26" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="107"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="134"/>
       <c r="E26" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="99"/>
-      <c r="G26" s="107" t="s">
-        <v>167</v>
+      <c r="F26" s="117"/>
+      <c r="G26" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H26" s="40">
         <v>1</v>
       </c>
       <c r="I26" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J26" s="44">
@@ -3132,25 +3194,26 @@
         <v>45139</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS26" s="6"/>
     </row>
-    <row r="27" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="63"/>
+    <row r="27" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="108"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="135"/>
       <c r="E27" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="100"/>
-      <c r="G27" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="H27" s="119">
+      <c r="F27" s="118"/>
+      <c r="G27" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="60">
         <v>1</v>
       </c>
       <c r="I27" s="16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J27" s="45">
@@ -3160,33 +3223,34 @@
         <v>45139</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS27" s="6"/>
     </row>
-    <row r="28" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="52" t="s">
+    <row r="28" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="106" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="130" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="130" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="128" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G28" s="120" t="s">
-        <v>167</v>
-      </c>
-      <c r="H28" s="121">
+      <c r="G28" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="62">
         <v>1</v>
       </c>
       <c r="I28" s="10">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J28" s="42">
@@ -3196,27 +3260,28 @@
         <v>45142</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AT28" s="6"/>
       <c r="AU28" s="6"/>
       <c r="AV28" s="6"/>
     </row>
-    <row r="29" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="60"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="56"/>
+    <row r="29" spans="2:48" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="107"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="129"/>
       <c r="F29" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="107" t="s">
-        <v>167</v>
+      <c r="G29" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H29" s="40">
         <v>1</v>
       </c>
       <c r="I29" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J29" s="44">
@@ -3232,23 +3297,24 @@
       <c r="AU29" s="6"/>
       <c r="AV29" s="6"/>
     </row>
-    <row r="30" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="60"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="56" t="s">
+    <row r="30" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="107"/>
+      <c r="C30" s="131"/>
+      <c r="D30" s="107"/>
+      <c r="E30" s="129" t="s">
         <v>80</v>
       </c>
       <c r="F30" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="107" t="s">
-        <v>167</v>
+      <c r="G30" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H30" s="40">
         <v>1</v>
       </c>
       <c r="I30" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J30" s="44">
@@ -3258,27 +3324,28 @@
         <v>45142</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AT30" s="6"/>
       <c r="AU30" s="6"/>
       <c r="AV30" s="6"/>
     </row>
-    <row r="31" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="60"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="56"/>
+    <row r="31" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="107"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="129"/>
       <c r="F31" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="107" t="s">
-        <v>167</v>
+      <c r="G31" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H31" s="40">
         <v>1</v>
       </c>
       <c r="I31" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J31" s="44">
@@ -3288,7 +3355,7 @@
         <v>45142</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O31" s="4" t="s">
         <v>117</v>
@@ -3297,21 +3364,22 @@
       <c r="AU31" s="6"/>
       <c r="AV31" s="6"/>
     </row>
-    <row r="32" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="60"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="56"/>
+    <row r="32" spans="2:48" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="107"/>
+      <c r="C32" s="131"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="129"/>
       <c r="F32" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="107" t="s">
-        <v>167</v>
+      <c r="G32" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H32" s="40">
         <v>1</v>
       </c>
       <c r="I32" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J32" s="44">
@@ -3321,27 +3389,28 @@
         <v>45142</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AT32" s="6"/>
       <c r="AU32" s="6"/>
       <c r="AV32" s="6"/>
     </row>
-    <row r="33" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="60"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="56"/>
+    <row r="33" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="107"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="129"/>
       <c r="F33" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="107" t="s">
-        <v>167</v>
+      <c r="G33" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H33" s="40">
         <v>1</v>
       </c>
       <c r="I33" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J33" s="44">
@@ -3351,29 +3420,30 @@
         <v>45142</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AT33" s="6"/>
       <c r="AU33" s="6"/>
       <c r="AV33" s="6"/>
     </row>
-    <row r="34" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="60"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="50" t="s">
+    <row r="34" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="107"/>
+      <c r="C34" s="131"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="75" t="s">
         <v>81</v>
       </c>
       <c r="F34" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G34" s="107" t="s">
-        <v>167</v>
+      <c r="G34" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H34" s="40">
         <v>1</v>
       </c>
       <c r="I34" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J34" s="44">
@@ -3389,21 +3459,22 @@
       <c r="AU34" s="6"/>
       <c r="AV34" s="6"/>
     </row>
-    <row r="35" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="60"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="51"/>
+    <row r="35" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="107"/>
+      <c r="C35" s="132"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="125"/>
       <c r="F35" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" s="122">
+      <c r="G35" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="63">
         <v>1</v>
       </c>
       <c r="I35" s="11">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J35" s="43">
@@ -3419,14 +3490,14 @@
       <c r="AU35" s="6"/>
       <c r="AV35" s="6"/>
     </row>
-    <row r="36" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="64" t="s">
+    <row r="36" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="72" t="s">
+      <c r="D36" s="119" t="s">
         <v>93</v>
       </c>
       <c r="E36" s="28" t="s">
@@ -3435,43 +3506,45 @@
       <c r="F36" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G36" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="H36" s="112">
-        <v>1</v>
-      </c>
-      <c r="I36" s="123">
-        <v>1</v>
-      </c>
-      <c r="J36" s="124">
+      <c r="G36" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="H36" s="56">
+        <v>1</v>
+      </c>
+      <c r="I36" s="64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="65">
         <v>45145</v>
       </c>
-      <c r="K36" s="124">
+      <c r="K36" s="65">
         <v>45145</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW36" s="6"/>
     </row>
-    <row r="37" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="50" t="s">
+    <row r="37" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="75" t="s">
         <v>95</v>
       </c>
       <c r="F37" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="107" t="s">
-        <v>167</v>
+      <c r="G37" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H37" s="40">
         <v>1</v>
       </c>
       <c r="I37" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J37" s="46">
@@ -3481,944 +3554,1198 @@
         <v>45145</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW37" s="6"/>
     </row>
-    <row r="38" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="50"/>
+    <row r="38" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="93"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="H38" s="119">
-        <v>1</v>
-      </c>
-      <c r="I38" s="125">
-        <v>1</v>
-      </c>
-      <c r="J38" s="126">
+      <c r="G38" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="60">
+        <v>1</v>
+      </c>
+      <c r="I38" s="66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J38" s="67">
         <v>45145</v>
       </c>
-      <c r="K38" s="126">
+      <c r="K38" s="67">
         <v>45145</v>
       </c>
       <c r="L38" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW38" s="6"/>
     </row>
-    <row r="39" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="50" t="s">
+    <row r="39" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="75" t="s">
         <v>96</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="120" t="s">
-        <v>167</v>
-      </c>
-      <c r="H39" s="121">
-        <v>1</v>
-      </c>
-      <c r="I39" s="127">
-        <v>1</v>
-      </c>
-      <c r="J39" s="128">
+      <c r="G39" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="H39" s="62">
+        <v>1</v>
+      </c>
+      <c r="I39" s="68">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="69">
         <v>45145</v>
       </c>
-      <c r="K39" s="128">
+      <c r="K39" s="69">
         <v>45145</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW39" s="6"/>
     </row>
-    <row r="40" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="50"/>
+    <row r="40" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="93"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="75"/>
       <c r="F40" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="H40" s="122">
-        <v>1</v>
-      </c>
-      <c r="I40" s="109">
-        <v>1</v>
-      </c>
-      <c r="J40" s="129">
+      <c r="G40" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="63">
+        <v>1</v>
+      </c>
+      <c r="I40" s="54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J40" s="70">
         <v>45145</v>
       </c>
-      <c r="K40" s="129">
+      <c r="K40" s="70">
         <v>45145</v>
       </c>
       <c r="L40" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW40" s="6"/>
     </row>
-    <row r="41" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="50" t="s">
+    <row r="41" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="75" t="s">
         <v>97</v>
       </c>
       <c r="F41" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="H41" s="112">
-        <v>1</v>
-      </c>
-      <c r="I41" s="123">
-        <v>1</v>
-      </c>
-      <c r="J41" s="124">
+      <c r="G41" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="H41" s="56">
+        <v>1</v>
+      </c>
+      <c r="I41" s="64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J41" s="65">
         <v>45145</v>
       </c>
-      <c r="K41" s="124">
+      <c r="K41" s="65">
         <v>45145</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW41" s="6"/>
     </row>
-    <row r="42" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="67"/>
+    <row r="42" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="105"/>
       <c r="F42" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="H42" s="119">
-        <v>1</v>
-      </c>
-      <c r="I42" s="125">
-        <v>1</v>
-      </c>
-      <c r="J42" s="126">
+      <c r="G42" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H42" s="60">
+        <v>1</v>
+      </c>
+      <c r="I42" s="66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J42" s="67">
         <v>45145</v>
       </c>
-      <c r="K42" s="126">
+      <c r="K42" s="67">
         <v>45145</v>
       </c>
       <c r="L42" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW42" s="6"/>
     </row>
-    <row r="43" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="94" t="s">
+    <row r="43" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="93"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="97" t="s">
+      <c r="E43" s="99" t="s">
         <v>126</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G43" s="120" t="s">
+      <c r="G43" s="61" t="s">
         <v>49</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I43" s="127"/>
-      <c r="J43" s="127"/>
-      <c r="K43" s="127"/>
+      <c r="I43" s="68" t="str">
+        <f>IF(OR(J43="",K43=""),"",K43-J43+1)</f>
+        <v/>
+      </c>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
       <c r="L43" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="86"/>
-      <c r="F44" s="101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="93"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="G44" s="107" t="s">
+      <c r="G44" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
+      <c r="I44" s="7" t="str">
+        <f t="shared" ref="I44:I57" si="1">IF(OR(J44="",K44=""),"",K44-J44+1)</f>
+        <v/>
+      </c>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
       <c r="L44" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="95"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="101" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="93"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="G45" s="107" t="s">
+      <c r="G45" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
+      <c r="I45" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
       <c r="L45" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="95"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="101" t="s">
+    <row r="46" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="93"/>
+      <c r="C46" s="93"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="G46" s="107" t="s">
+      <c r="G46" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
+      <c r="I46" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
       <c r="L46" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="65"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="95"/>
-      <c r="E47" s="86"/>
-      <c r="F47" s="101" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="2:49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="93"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="G47" s="107" t="s">
+      <c r="G47" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+      <c r="I47" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
       <c r="L47" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B48" s="65"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="102" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="2:49" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="93"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="G48" s="108" t="s">
+      <c r="G48" s="53" t="s">
         <v>49</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I48" s="109"/>
-      <c r="J48" s="109"/>
-      <c r="K48" s="109"/>
+      <c r="I48" s="54" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J48" s="70"/>
+      <c r="K48" s="70"/>
       <c r="L48" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="95"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="93"/>
+      <c r="C49" s="93"/>
+      <c r="D49" s="96"/>
       <c r="E49" s="38" t="s">
         <v>120</v>
       </c>
       <c r="F49" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="G49" s="130" t="s">
+      <c r="G49" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="H49" s="131" t="s">
+      <c r="H49" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="I49" s="132"/>
-      <c r="J49" s="132"/>
-      <c r="K49" s="132"/>
-      <c r="L49" s="133" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="95"/>
-      <c r="E50" s="85" t="s">
+      <c r="I49" s="73" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J49" s="137"/>
+      <c r="K49" s="137"/>
+      <c r="L49" s="74" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="93"/>
+      <c r="C50" s="93"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="83" t="s">
         <v>121</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="G50" s="120" t="s">
+      <c r="G50" s="61" t="s">
         <v>49</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I50" s="127"/>
-      <c r="J50" s="127"/>
-      <c r="K50" s="127"/>
+      <c r="I50" s="68" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
       <c r="L50" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="65"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="95"/>
-      <c r="E51" s="86"/>
-      <c r="F51" s="101" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="93"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="G51" s="107" t="s">
+      <c r="G51" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
+      <c r="I51" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
       <c r="L51" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="86"/>
-      <c r="F52" s="104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="93"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="G52" s="118" t="s">
+      <c r="G52" s="59" t="s">
         <v>49</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I52" s="125"/>
-      <c r="J52" s="125"/>
-      <c r="K52" s="125"/>
+      <c r="I52" s="66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J52" s="67"/>
+      <c r="K52" s="67"/>
       <c r="L52" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="134"/>
-      <c r="E53" s="82" t="s">
-        <v>174</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="93"/>
+      <c r="C53" s="93"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="76" t="s">
+        <v>173</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="G53" s="120" t="s">
+        <v>182</v>
+      </c>
+      <c r="G53" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="H53" s="121">
-        <v>1</v>
-      </c>
-      <c r="I53" s="127"/>
-      <c r="J53" s="127"/>
-      <c r="K53" s="127"/>
+      <c r="H53" s="62">
+        <v>1</v>
+      </c>
+      <c r="I53" s="68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J53" s="69">
+        <v>45150</v>
+      </c>
+      <c r="K53" s="69">
+        <v>45150</v>
+      </c>
       <c r="L53" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="134"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="G54" s="107" t="s">
+    <row r="54" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="93"/>
+      <c r="C54" s="93"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="G54" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="H54" s="56">
+        <v>1</v>
+      </c>
+      <c r="I54" s="64">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J54" s="65">
+        <v>45150</v>
+      </c>
+      <c r="K54" s="65">
+        <v>45151</v>
+      </c>
+      <c r="L54" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
+      <c r="P54" s="47"/>
+      <c r="Q54" s="47"/>
+      <c r="R54" s="47"/>
+      <c r="S54" s="47"/>
+      <c r="T54" s="47"/>
+      <c r="U54" s="47"/>
+      <c r="V54" s="47"/>
+      <c r="W54" s="47"/>
+      <c r="X54" s="47"/>
+      <c r="Y54" s="47"/>
+      <c r="Z54" s="47"/>
+      <c r="AA54" s="47"/>
+      <c r="AB54" s="47"/>
+      <c r="AC54" s="47"/>
+      <c r="AD54" s="47"/>
+      <c r="AE54" s="47"/>
+      <c r="AF54" s="47"/>
+      <c r="AG54" s="47"/>
+      <c r="AH54" s="47"/>
+      <c r="AI54" s="47"/>
+      <c r="AJ54" s="47"/>
+      <c r="AK54" s="47"/>
+      <c r="AL54" s="47"/>
+      <c r="AM54" s="47"/>
+      <c r="AN54" s="47"/>
+      <c r="AO54" s="47"/>
+      <c r="AP54" s="47"/>
+      <c r="AQ54" s="47"/>
+      <c r="AR54" s="47"/>
+      <c r="AS54" s="47"/>
+      <c r="AT54" s="47"/>
+      <c r="AU54" s="47"/>
+      <c r="AV54" s="47"/>
+      <c r="AW54" s="47"/>
+      <c r="AX54" s="47"/>
+      <c r="AY54" s="47"/>
+      <c r="AZ54" s="47"/>
+      <c r="BA54" s="47"/>
+      <c r="BB54" s="47"/>
+      <c r="BC54" s="47"/>
+      <c r="BD54" s="47"/>
+      <c r="BE54" s="47"/>
+      <c r="BF54" s="47"/>
+      <c r="BG54" s="47"/>
+      <c r="BH54" s="47"/>
+      <c r="BI54" s="47"/>
+      <c r="BJ54" s="47"/>
+      <c r="BK54" s="47"/>
+      <c r="BL54" s="47"/>
+      <c r="BM54" s="47"/>
+      <c r="BN54" s="47"/>
+      <c r="BO54" s="47"/>
+      <c r="BP54" s="47"/>
+      <c r="BQ54" s="47"/>
+      <c r="BR54" s="47"/>
+      <c r="BS54" s="47"/>
+    </row>
+    <row r="55" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="93"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G55" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H54" s="40">
-        <v>1</v>
-      </c>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="65"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="134"/>
-      <c r="E55" s="83"/>
-      <c r="F55" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="G55" s="107" t="s">
-        <v>49</v>
-      </c>
       <c r="H55" s="40">
         <v>1</v>
       </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
+      <c r="I55" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J55" s="46">
+        <v>45151</v>
+      </c>
+      <c r="K55" s="46">
+        <v>45152</v>
+      </c>
       <c r="L55" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="134"/>
-      <c r="E56" s="84"/>
-      <c r="F56" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="G56" s="118" t="s">
+    <row r="56" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="93"/>
+      <c r="C56" s="93"/>
+      <c r="D56" s="97"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="G56" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="119">
-        <v>1</v>
-      </c>
-      <c r="I56" s="125"/>
-      <c r="J56" s="125"/>
-      <c r="K56" s="125"/>
-      <c r="L56" s="20" t="s">
+      <c r="H56" s="40">
+        <v>1</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J56" s="46">
+        <v>45153</v>
+      </c>
+      <c r="K56" s="46">
+        <v>45154</v>
+      </c>
+      <c r="L56" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="65"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="95"/>
-      <c r="E57" s="86" t="s">
+    <row r="57" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="93"/>
+      <c r="C57" s="93"/>
+      <c r="D57" s="97"/>
+      <c r="E57" s="78"/>
+      <c r="F57" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G57" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57" s="60">
+        <v>1</v>
+      </c>
+      <c r="I57" s="66">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J57" s="67">
+        <v>45151</v>
+      </c>
+      <c r="K57" s="67">
+        <v>45153</v>
+      </c>
+      <c r="L57" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="93"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="G58" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I58" s="136" t="str">
+        <f>IF(OR(J58="",K58=""),"",K58-J58+1)</f>
+        <v/>
+      </c>
+      <c r="J58" s="69"/>
+      <c r="K58" s="69"/>
+      <c r="L58" s="12"/>
+    </row>
+    <row r="59" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="96"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="G59" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I59" s="54" t="str">
+        <f t="shared" ref="I59:I78" si="2">IF(OR(J59="",K59=""),"",K59-J59+1)</f>
+        <v/>
+      </c>
+      <c r="J59" s="70"/>
+      <c r="K59" s="70"/>
+      <c r="L59" s="14"/>
+    </row>
+    <row r="60" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="96"/>
+      <c r="E60" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="F57" s="103" t="s">
-        <v>177</v>
-      </c>
-      <c r="G57" s="120" t="s">
-        <v>72</v>
-      </c>
-      <c r="H57" s="10" t="s">
+      <c r="F60" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="G60" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="I57" s="127"/>
-      <c r="J57" s="127"/>
-      <c r="K57" s="127"/>
-      <c r="L57" s="12"/>
-    </row>
-    <row r="58" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="95"/>
-      <c r="E58" s="87"/>
-      <c r="F58" s="102" t="s">
-        <v>178</v>
-      </c>
-      <c r="G58" s="108" t="s">
-        <v>72</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I58" s="109"/>
-      <c r="J58" s="109"/>
-      <c r="K58" s="109"/>
-      <c r="L58" s="14"/>
-    </row>
-    <row r="59" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="65"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="95"/>
-      <c r="E59" s="85" t="s">
-        <v>176</v>
-      </c>
-      <c r="F59" s="103" t="s">
+      <c r="I60" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J60" s="65"/>
+      <c r="K60" s="65"/>
+      <c r="L60" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="93"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="84"/>
+      <c r="F61" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="G59" s="111" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" s="113" t="s">
-        <v>98</v>
-      </c>
-      <c r="I59" s="123"/>
-      <c r="J59" s="123"/>
-      <c r="K59" s="123"/>
-      <c r="L59" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="65"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="95"/>
-      <c r="E60" s="86"/>
-      <c r="F60" s="101" t="s">
-        <v>180</v>
-      </c>
-      <c r="G60" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="65"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="95"/>
-      <c r="E61" s="86"/>
-      <c r="F61" s="101" t="s">
-        <v>181</v>
-      </c>
-      <c r="G61" s="107" t="s">
+      <c r="G61" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H61" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
+      <c r="I61" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
       <c r="L61" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B62" s="65"/>
-      <c r="C62" s="65"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
       <c r="D62" s="96"/>
-      <c r="E62" s="87"/>
-      <c r="F62" s="102" t="s">
-        <v>182</v>
-      </c>
-      <c r="G62" s="108" t="s">
+      <c r="E62" s="84"/>
+      <c r="F62" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G62" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H62" s="11" t="s">
+      <c r="H62" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I62" s="109"/>
-      <c r="J62" s="109"/>
-      <c r="K62" s="109"/>
-      <c r="L62" s="14" t="s">
+      <c r="I62" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="93"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="G63" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I63" s="54" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70"/>
+      <c r="L63" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="65"/>
-      <c r="C63" s="65"/>
-      <c r="D63" s="91" t="s">
+    <row r="64" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="93"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="E63" s="88" t="s">
+      <c r="E64" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F64" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="G63" s="111" t="s">
+      <c r="G64" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="H63" s="113" t="s">
+      <c r="H64" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="I63" s="123"/>
-      <c r="J63" s="123"/>
-      <c r="K63" s="123"/>
-      <c r="L63" s="19"/>
-    </row>
-    <row r="64" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B64" s="65"/>
-      <c r="C64" s="65"/>
-      <c r="D64" s="92"/>
-      <c r="E64" s="89"/>
-      <c r="F64" s="101" t="s">
+      <c r="I64" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J64" s="65"/>
+      <c r="K64" s="65"/>
+      <c r="L64" s="19"/>
+    </row>
+    <row r="65" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="93"/>
+      <c r="C65" s="93"/>
+      <c r="D65" s="90"/>
+      <c r="E65" s="87"/>
+      <c r="F65" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="G64" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="65"/>
-      <c r="C65" s="65"/>
-      <c r="D65" s="92"/>
-      <c r="E65" s="89"/>
-      <c r="F65" s="101" t="s">
-        <v>137</v>
-      </c>
-      <c r="G65" s="107" t="s">
+      <c r="G65" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H65" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
+      <c r="I65" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J65" s="46"/>
+      <c r="K65" s="46"/>
       <c r="L65" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B66" s="65"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="92"/>
-      <c r="E66" s="89"/>
-      <c r="F66" s="101" t="s">
-        <v>138</v>
-      </c>
-      <c r="G66" s="107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="93"/>
+      <c r="C66" s="93"/>
+      <c r="D66" s="90"/>
+      <c r="E66" s="87"/>
+      <c r="F66" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G66" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H66" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
+      <c r="I66" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
       <c r="L66" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="65"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="92"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="101" t="s">
-        <v>139</v>
-      </c>
-      <c r="G67" s="107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="93"/>
+      <c r="C67" s="93"/>
+      <c r="D67" s="90"/>
+      <c r="E67" s="87"/>
+      <c r="F67" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="G67" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H67" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
+      <c r="I67" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J67" s="46"/>
+      <c r="K67" s="46"/>
       <c r="L67" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B68" s="65"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="89"/>
-      <c r="F68" s="101" t="s">
-        <v>140</v>
-      </c>
-      <c r="G68" s="107" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="93"/>
+      <c r="C68" s="93"/>
+      <c r="D68" s="90"/>
+      <c r="E68" s="87"/>
+      <c r="F68" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G68" s="52" t="s">
         <v>49</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
+      <c r="I68" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J68" s="46"/>
+      <c r="K68" s="46"/>
       <c r="L68" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="93"/>
+      <c r="C69" s="93"/>
+      <c r="D69" s="90"/>
+      <c r="E69" s="87"/>
+      <c r="F69" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G69" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I69" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J69" s="46"/>
+      <c r="K69" s="46"/>
+      <c r="L69" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="93"/>
+      <c r="C70" s="93"/>
+      <c r="D70" s="90"/>
+      <c r="E70" s="87"/>
+      <c r="F70" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="G70" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="H70" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="I70" s="66" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J70" s="67"/>
+      <c r="K70" s="67"/>
+      <c r="L70" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="M70" s="47"/>
+      <c r="N70" s="47"/>
+      <c r="O70" s="47"/>
+      <c r="P70" s="47"/>
+      <c r="Q70" s="47"/>
+      <c r="R70" s="47"/>
+      <c r="S70" s="47"/>
+      <c r="T70" s="47"/>
+      <c r="U70" s="47"/>
+      <c r="V70" s="47"/>
+      <c r="W70" s="47"/>
+      <c r="X70" s="47"/>
+      <c r="Y70" s="47"/>
+      <c r="Z70" s="47"/>
+      <c r="AA70" s="47"/>
+      <c r="AB70" s="47"/>
+      <c r="AC70" s="47"/>
+      <c r="AD70" s="47"/>
+      <c r="AE70" s="47"/>
+      <c r="AF70" s="47"/>
+      <c r="AG70" s="47"/>
+      <c r="AH70" s="47"/>
+      <c r="AI70" s="47"/>
+      <c r="AJ70" s="47"/>
+      <c r="AK70" s="47"/>
+      <c r="AL70" s="47"/>
+      <c r="AM70" s="47"/>
+      <c r="AN70" s="47"/>
+      <c r="AO70" s="47"/>
+      <c r="AP70" s="47"/>
+      <c r="AQ70" s="47"/>
+      <c r="AR70" s="47"/>
+      <c r="AS70" s="47"/>
+      <c r="AT70" s="47"/>
+      <c r="AU70" s="47"/>
+      <c r="AV70" s="47"/>
+      <c r="AW70" s="47"/>
+      <c r="AX70" s="47"/>
+      <c r="AY70" s="47"/>
+      <c r="AZ70" s="47"/>
+      <c r="BA70" s="47"/>
+      <c r="BB70" s="47"/>
+      <c r="BC70" s="47"/>
+      <c r="BD70" s="47"/>
+      <c r="BE70" s="47"/>
+      <c r="BF70" s="47"/>
+      <c r="BG70" s="47"/>
+      <c r="BH70" s="47"/>
+      <c r="BI70" s="47"/>
+      <c r="BJ70" s="47"/>
+      <c r="BK70" s="47"/>
+      <c r="BL70" s="47"/>
+      <c r="BM70" s="47"/>
+      <c r="BN70" s="47"/>
+      <c r="BO70" s="47"/>
+      <c r="BP70" s="47"/>
+      <c r="BQ70" s="47"/>
+      <c r="BR70" s="47"/>
+      <c r="BS70" s="47"/>
+    </row>
+    <row r="71" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="93"/>
+      <c r="C71" s="93"/>
+      <c r="D71" s="90"/>
+      <c r="E71" s="88"/>
+      <c r="F71" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G71" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="H71" s="60">
+        <v>0.9</v>
+      </c>
+      <c r="I71" s="66" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J71" s="67">
+        <v>45150</v>
+      </c>
+      <c r="K71" s="67"/>
+      <c r="L71" s="20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="93"/>
+      <c r="C72" s="93"/>
+      <c r="D72" s="90"/>
+      <c r="E72" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I72" s="68" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J72" s="69"/>
+      <c r="K72" s="69"/>
+      <c r="L72" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="93"/>
+      <c r="C73" s="93"/>
+      <c r="D73" s="90"/>
+      <c r="E73" s="85"/>
+      <c r="F73" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I73" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J73" s="46"/>
+      <c r="K73" s="46"/>
+      <c r="L73" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="94"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="91"/>
+      <c r="E74" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="G74" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I74" s="54" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J74" s="70"/>
+      <c r="K74" s="70"/>
+      <c r="L74" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B69" s="65"/>
-      <c r="C69" s="65"/>
-      <c r="D69" s="92"/>
-      <c r="E69" s="90"/>
-      <c r="F69" s="104" t="s">
-        <v>141</v>
-      </c>
-      <c r="G69" s="118" t="s">
-        <v>49</v>
-      </c>
-      <c r="H69" s="16" t="s">
+    <row r="75" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="83" t="s">
+        <v>147</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="F75" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="G75" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="H75" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="I69" s="125"/>
-      <c r="J69" s="125"/>
-      <c r="K69" s="125"/>
-      <c r="L69" s="20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B70" s="65"/>
-      <c r="C70" s="65"/>
-      <c r="D70" s="92"/>
-      <c r="E70" s="85" t="s">
-        <v>142</v>
-      </c>
-      <c r="F70" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G70" s="120" t="s">
-        <v>49</v>
-      </c>
-      <c r="H70" s="10" t="s">
+      <c r="I75" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J75" s="65"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="77"/>
+      <c r="C76" s="77"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G76" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="H76" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I70" s="127"/>
-      <c r="J70" s="127"/>
-      <c r="K70" s="127"/>
-      <c r="L70" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B71" s="65"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="92"/>
-      <c r="E71" s="87"/>
-      <c r="F71" s="101" t="s">
-        <v>144</v>
-      </c>
-      <c r="G71" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="H71" s="9" t="s">
+      <c r="I76" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J76" s="46"/>
+      <c r="K76" s="46"/>
+      <c r="L76" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="2:71" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="77"/>
+      <c r="C77" s="77"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F77" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="G77" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="H77" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B72" s="66"/>
-      <c r="C72" s="66"/>
-      <c r="D72" s="93"/>
-      <c r="E72" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="F72" s="104" t="s">
-        <v>146</v>
-      </c>
-      <c r="G72" s="108" t="s">
-        <v>49</v>
-      </c>
-      <c r="H72" s="11" t="s">
+      <c r="I77" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J77" s="46"/>
+      <c r="K77" s="46"/>
+      <c r="L77" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="2:71" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="78"/>
+      <c r="C78" s="78"/>
+      <c r="D78" s="85"/>
+      <c r="E78" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="G78" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="H78" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="109"/>
-      <c r="J72" s="109"/>
-      <c r="K72" s="109"/>
-      <c r="L72" s="14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B73" s="82" t="s">
-        <v>118</v>
-      </c>
-      <c r="C73" s="82" t="s">
-        <v>147</v>
-      </c>
-      <c r="D73" s="85" t="s">
-        <v>148</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="F73" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="G73" s="111" t="s">
-        <v>71</v>
-      </c>
-      <c r="H73" s="113" t="s">
-        <v>98</v>
-      </c>
-      <c r="I73" s="123"/>
-      <c r="J73" s="123"/>
-      <c r="K73" s="123"/>
-      <c r="L73" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B74" s="83"/>
-      <c r="C74" s="83"/>
-      <c r="D74" s="86"/>
-      <c r="E74" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F74" s="101" t="s">
-        <v>152</v>
-      </c>
-      <c r="G74" s="107" t="s">
-        <v>71</v>
-      </c>
-      <c r="H74" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I74" s="7"/>
-      <c r="J74" s="7"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B75" s="83"/>
-      <c r="C75" s="83"/>
-      <c r="D75" s="86"/>
-      <c r="E75" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F75" s="101" t="s">
-        <v>154</v>
-      </c>
-      <c r="G75" s="107" t="s">
-        <v>71</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I75" s="7"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B76" s="84"/>
-      <c r="C76" s="84"/>
-      <c r="D76" s="87"/>
-      <c r="E76" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="F76" s="102" t="s">
-        <v>156</v>
-      </c>
-      <c r="G76" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I76" s="109"/>
-      <c r="J76" s="109"/>
-      <c r="K76" s="109"/>
-      <c r="L76" s="14" t="s">
-        <v>161</v>
+      <c r="I78" s="54" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J78" s="70"/>
+      <c r="K78" s="70"/>
+      <c r="L78" s="14" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="D73:D76"/>
-    <mergeCell ref="E63:E69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="D63:D72"/>
-    <mergeCell ref="C36:C72"/>
-    <mergeCell ref="B36:B72"/>
-    <mergeCell ref="D43:D62"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="BL11:BR11"/>
-    <mergeCell ref="AJ11:AP11"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="AS11:AW11"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="N10:AR10"/>
-    <mergeCell ref="O11:U11"/>
-    <mergeCell ref="V11:AB11"/>
-    <mergeCell ref="AC11:AI11"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="F13:F27"/>
-    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="BS11:BW11"/>
+    <mergeCell ref="AX11:BD11"/>
+    <mergeCell ref="BE11:BK11"/>
     <mergeCell ref="B28:B35"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
@@ -4435,9 +4762,50 @@
     <mergeCell ref="C22:C27"/>
     <mergeCell ref="D22:D27"/>
     <mergeCell ref="D15:D21"/>
-    <mergeCell ref="BS11:BW11"/>
-    <mergeCell ref="AX11:BD11"/>
-    <mergeCell ref="BE11:BK11"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="N10:AR10"/>
+    <mergeCell ref="O11:U11"/>
+    <mergeCell ref="V11:AB11"/>
+    <mergeCell ref="AC11:AI11"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F13:F27"/>
+    <mergeCell ref="BL11:BR11"/>
+    <mergeCell ref="AJ11:AP11"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="AS11:AW11"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E64:E71"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="D64:D74"/>
+    <mergeCell ref="C36:C74"/>
+    <mergeCell ref="B36:B74"/>
+    <mergeCell ref="D43:D63"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>